<commit_message>
update video part 3
</commit_message>
<xml_diff>
--- a/SampleTables.xlsx
+++ b/SampleTables.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Playground\Videos\BlazorForKidsSampleDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B253B1-96E2-4BDD-B0F0-CEB854258E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D508E75D-F797-4105-B926-7533A54BDEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72000" yWindow="2190" windowWidth="28800" windowHeight="11235" xr2:uid="{A6B92A3C-27A4-46ED-B3C6-527E9B216EC5}"/>
+    <workbookView xWindow="71880" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{A6B92A3C-27A4-46ED-B3C6-527E9B216EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
     <sheet name="Departments" sheetId="2" r:id="rId2"/>
+    <sheet name="EmployeeInfo" sheetId="4" r:id="rId3"/>
+    <sheet name="EmployeeInfoForm" sheetId="5" r:id="rId4"/>
+    <sheet name="Training Documents" sheetId="6" r:id="rId5"/>
+    <sheet name="EmployeeTrainingDocuments" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="82">
   <si>
     <t>Id</t>
   </si>
@@ -127,13 +131,185 @@
   </si>
   <si>
     <t>Last Name 11</t>
+  </si>
+  <si>
+    <t>DateOfHire</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>BadgeNumber</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>🤵</t>
+  </si>
+  <si>
+    <t>IsActive</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>ℹ️Info</t>
+  </si>
+  <si>
+    <t>ℹ️ Info</t>
+  </si>
+  <si>
+    <t>Date of Hire</t>
+  </si>
+  <si>
+    <t>Badge Number</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">☑️  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IsActive</t>
+    </r>
+  </si>
+  <si>
+    <t>Employee Info Layout</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>DocumentFile</t>
+  </si>
+  <si>
+    <t>Document 1</t>
+  </si>
+  <si>
+    <t>Document 2</t>
+  </si>
+  <si>
+    <t>Document 3</t>
+  </si>
+  <si>
+    <t>Document 4</t>
+  </si>
+  <si>
+    <t>Document 5</t>
+  </si>
+  <si>
+    <t>Document 6</t>
+  </si>
+  <si>
+    <t>Document 7</t>
+  </si>
+  <si>
+    <t>Document 8</t>
+  </si>
+  <si>
+    <t>Document 9</t>
+  </si>
+  <si>
+    <t>Document 10</t>
+  </si>
+  <si>
+    <t>Document 11</t>
+  </si>
+  <si>
+    <t>📄file1</t>
+  </si>
+  <si>
+    <t>📄file2</t>
+  </si>
+  <si>
+    <t>📄file3</t>
+  </si>
+  <si>
+    <t>📄file4</t>
+  </si>
+  <si>
+    <t>📄file5</t>
+  </si>
+  <si>
+    <t>📄file6</t>
+  </si>
+  <si>
+    <t>📄file7</t>
+  </si>
+  <si>
+    <t>📄file8</t>
+  </si>
+  <si>
+    <t>📄file9</t>
+  </si>
+  <si>
+    <t>📄file10</t>
+  </si>
+  <si>
+    <t>📄file11</t>
+  </si>
+  <si>
+    <t>Training Documents</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
+  </si>
+  <si>
+    <t>DocumentId</t>
+  </si>
+  <si>
+    <t>TrainingStatus</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Employee Training Documents</t>
+  </si>
+  <si>
+    <t>DepartmentId</t>
+  </si>
+  <si>
+    <t>DepartmentDocuments</t>
+  </si>
+  <si>
+    <t>One document can be for many departments</t>
+  </si>
+  <si>
+    <t>A department can have many documents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +323,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="3" tint="0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,8 +388,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -196,17 +453,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -220,6 +529,916 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D52B86F8-061F-7954-CFA8-9E7A12BB736A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2190750" y="5153025"/>
+          <a:ext cx="1466850" cy="1152525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>TrainingDocument</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F49D928-873E-AF78-04CD-920FC9634890}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4724400" y="5143500"/>
+          <a:ext cx="1466850" cy="1152525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>Department</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1085851</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connector: Elbow 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6388C6E7-9D3D-5828-4629-6DF7DAE92489}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="0"/>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="4186238" y="3881438"/>
+          <a:ext cx="9525" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2500000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1085851</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connector: Elbow 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F7B5EEE-C801-CFA4-2919-4557B0AD41A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="2" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4186238" y="5033962"/>
+          <a:ext cx="9525" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2500000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A324461A-0D7C-8281-F75C-299618B82E8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7658100" y="6372225"/>
+          <a:ext cx="1628775" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Document 1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFC935E3-20F1-02E8-354B-2D44AAA76062}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7667625" y="7267575"/>
+          <a:ext cx="1628775" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Document 2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6505B238-ACB7-E99B-5CE7-3FAF756123E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7677150" y="8134350"/>
+          <a:ext cx="1628775" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Document 3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1552575</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F7C34E-8E19-4442-105B-E8C649DA91DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10144125" y="6343650"/>
+          <a:ext cx="1628775" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Production</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B67192-65D5-95F3-4A65-405BD1574886}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10153650" y="7277100"/>
+          <a:ext cx="1628775" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Quality</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{175CF97C-E833-D9FF-DA61-938BC1C0A6E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10163175" y="8143875"/>
+          <a:ext cx="1628775" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Sales</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1552575</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBC6E761-1CC3-6CBA-6B8F-2DBC908B2975}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="3"/>
+          <a:endCxn id="11" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9286875" y="6643688"/>
+          <a:ext cx="857250" cy="28575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>147638</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{685A7F29-9B2D-4DAE-9A74-C4902E021A49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9277350" y="7548563"/>
+          <a:ext cx="857250" cy="28575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25772F82-FA18-4DA1-B84F-5E0AA39CC386}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9305925" y="8453438"/>
+          <a:ext cx="857250" cy="28575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AEEFD39-59D8-440F-AEFE-AD8933D2FA7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9315450" y="7753350"/>
+          <a:ext cx="819150" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32EC1CD3-7328-4A1E-BE30-987C59B88A57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9315450" y="6848475"/>
+          <a:ext cx="819150" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -539,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E407AE-109E-426C-B3E4-5DB626D5FFC6}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,9 +1769,10 @@
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,8 +1785,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -579,8 +1802,11 @@
       <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -593,8 +1819,11 @@
       <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -607,8 +1836,11 @@
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -621,8 +1853,11 @@
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -635,8 +1870,11 @@
       <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -649,8 +1887,11 @@
       <c r="D7" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -663,8 +1904,11 @@
       <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -677,8 +1921,11 @@
       <c r="D9" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -691,8 +1938,11 @@
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -705,8 +1955,11 @@
       <c r="D11" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -719,9 +1972,16 @@
       <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="E12" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" location="EmployeeInfo!A1" display="ℹ️Info" xr:uid="{DA3AD118-8749-445F-90DF-B73A3C229FEA}"/>
+    <hyperlink ref="E3:E12" location="EmployeeInfo!A1" display="ℹ️Info" xr:uid="{58E2380E-E4D0-4969-9882-CA2532401394}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -787,4 +2047,1454 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C565AA-EAB3-41E4-B3D5-CE9D3CF9C2E4}">
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="18" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>36655</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="6">
+        <f ca="1">RANDBETWEEN(1000,2000)</f>
+        <v>1365</v>
+      </c>
+      <c r="F2" s="7">
+        <f ca="1">RANDBETWEEN(10000,20000)</f>
+        <v>17022</v>
+      </c>
+      <c r="G2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>37087</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E11" ca="1" si="0">RANDBETWEEN(1000,2000)</f>
+        <v>1377</v>
+      </c>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F11" ca="1" si="1">RANDBETWEEN(10000,20000)</f>
+        <v>12958</v>
+      </c>
+      <c r="G3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>37519</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1782</v>
+      </c>
+      <c r="F4" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>18508</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>37951</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1632</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>13418</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>38383</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1068</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>19591</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>38815</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1002</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>17263</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>39247</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1284</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>19317</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="19"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>39679</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1964</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>11821</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="19"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>40111</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1548</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>14542</v>
+      </c>
+      <c r="G10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>40543</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1845</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>11407</v>
+      </c>
+      <c r="G11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="13"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="13"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+    </row>
+    <row r="16" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J16" s="12"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="13"/>
+    </row>
+    <row r="17" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J17" s="12"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="L16:P16"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="O14:P14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236B11E6-B56E-45D1-ABD0-C9238EFC5A4D}">
+  <dimension ref="A1:AA32"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AD12" sqref="AD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>36655</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="6">
+        <f ca="1">RANDBETWEEN(1000,2000)</f>
+        <v>1502</v>
+      </c>
+      <c r="F2" s="7">
+        <f ca="1">RANDBETWEEN(10000,20000)</f>
+        <v>19841</v>
+      </c>
+      <c r="G2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>37087</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E11" ca="1" si="0">RANDBETWEEN(1000,2000)</f>
+        <v>1044</v>
+      </c>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F11" ca="1" si="1">RANDBETWEEN(10000,20000)</f>
+        <v>17578</v>
+      </c>
+      <c r="G3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>37519</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1318</v>
+      </c>
+      <c r="F4" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>14122</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>37951</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1348</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>18174</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>38383</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1870</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>16011</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>38815</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1486</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>19270</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>39247</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1284</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>11833</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="19"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>39679</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1612</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>13272</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="19"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>40111</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1853</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>12654</v>
+      </c>
+      <c r="G10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>40543</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1666</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>14843</v>
+      </c>
+      <c r="G11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+    </row>
+    <row r="16" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J16" s="12"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+    </row>
+    <row r="17" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="J17" s="12"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+    </row>
+    <row r="18" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+    </row>
+    <row r="21" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U22" s="16"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+    </row>
+    <row r="23" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U23" s="16"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+    </row>
+    <row r="24" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U24" s="16"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+    </row>
+    <row r="25" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U25" s="16"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="15"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="15"/>
+    </row>
+    <row r="26" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U26" s="16"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="15"/>
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="15"/>
+      <c r="AA26" s="15"/>
+    </row>
+    <row r="27" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U27" s="16"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="15"/>
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="15"/>
+      <c r="AA27" s="15"/>
+    </row>
+    <row r="28" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U28" s="16"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="15"/>
+    </row>
+    <row r="29" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U29" s="16"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="15"/>
+      <c r="Y29" s="15"/>
+      <c r="Z29" s="15"/>
+      <c r="AA29" s="15"/>
+    </row>
+    <row r="30" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U30" s="16"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="15"/>
+    </row>
+    <row r="31" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U31" s="16"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="15"/>
+      <c r="X31" s="15"/>
+      <c r="Y31" s="15"/>
+      <c r="Z31" s="15"/>
+      <c r="AA31" s="15"/>
+    </row>
+    <row r="32" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="U32" s="16"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="15"/>
+      <c r="X32" s="15"/>
+      <c r="Y32" s="15"/>
+      <c r="Z32" s="15"/>
+      <c r="AA32" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="L16:P16"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="O14:P14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4E9716-7216-4A0F-B6D5-89CDA154AE49}">
+  <dimension ref="E7:K36"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E7" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="J8" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="2">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="2">
+        <v>7</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <v>8</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <v>9</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E20" s="2">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="J8:K8"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CA153F-7F38-44A8-A0F6-3B0823E5E99C}">
+  <dimension ref="C4:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>